<commit_message>
final database1 and ER dig
</commit_message>
<xml_diff>
--- a/DataBase/FinalDatabase_and_ER.xlsx
+++ b/DataBase/FinalDatabase_and_ER.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abc\Desktop\AgroGet\DataBase\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="2"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Final Database" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Populated-DB" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="ER-Dia" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="shridhar" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Sumit" sheetId="5" r:id="rId8"/>
+    <sheet name="Final Database" sheetId="1" r:id="rId1"/>
+    <sheet name="Populated-DB" sheetId="2" r:id="rId2"/>
+    <sheet name="ER-Dia" sheetId="3" r:id="rId3"/>
+    <sheet name="shridhar" sheetId="4" r:id="rId4"/>
+    <sheet name="Sumit" sheetId="5" r:id="rId5"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataSignature="AMtx7mi0Q0PqaFw5yWZ1KNNXMNnG7UpVGQ=="/>
@@ -20,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="277">
   <si>
     <t>farmer_info_tbl</t>
   </si>
@@ -845,84 +853,95 @@
   </si>
   <si>
     <t>Farmer_Info_Tbl</t>
+  </si>
+  <si>
+    <t>farmer_Password</t>
+  </si>
+  <si>
+    <t>farmer_Pincode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
   <fonts count="14">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Docs-Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Docs-Calibri"/>
     </font>
@@ -932,7 +951,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1002,12 +1021,19 @@
     </fill>
   </fills>
   <borders count="9">
-    <border/>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -1022,28 +1048,37 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left/>
+      <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -1053,299 +1088,223 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
+      <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right/>
+      <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="80">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="1" fillId="4" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="8" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="7" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="9" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="9" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="9" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="9" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="9" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="3" fillId="7" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="7" fontId="10" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="7" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="9" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="9" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="9" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="5" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="10" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="11" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="12" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="2" fillId="12" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="12" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="12" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="5" fillId="12" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="6" fillId="12" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="12" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="12" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="12" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="0" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="6" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="9" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
-  <xdr:oneCellAnchor>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>406555</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>116158</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="8458200" cy="9010650"/>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>209086</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>69695</xdr:rowOff>
+    </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1370671" y="302012"/>
+          <a:ext cx="9443689" cy="11104756"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
       </xdr:spPr>
     </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>184</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="8448675" cy="8315325"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1535,39 +1494,41 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V946"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="27.86"/>
-    <col customWidth="1" min="2" max="2" width="19.71"/>
-    <col customWidth="1" min="3" max="3" width="22.86"/>
-    <col customWidth="1" min="4" max="4" width="22.0"/>
-    <col customWidth="1" min="5" max="5" width="15.14"/>
-    <col customWidth="1" min="6" max="6" width="17.71"/>
-    <col customWidth="1" min="7" max="7" width="23.14"/>
-    <col customWidth="1" min="8" max="8" width="25.29"/>
-    <col customWidth="1" min="9" max="9" width="18.43"/>
-    <col customWidth="1" min="10" max="10" width="24.29"/>
-    <col customWidth="1" min="11" max="11" width="8.71"/>
-    <col customWidth="1" min="12" max="12" width="13.43"/>
-    <col customWidth="1" min="13" max="13" width="20.43"/>
-    <col customWidth="1" min="14" max="26" width="8.71"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" customWidth="1"/>
+    <col min="8" max="8" width="25.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="10" max="10" width="24.28515625" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="20.42578125" customWidth="1"/>
+    <col min="14" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1"/>
-    <row r="2" ht="14.25" customHeight="1"/>
-    <row r="3" ht="14.25" customHeight="1"/>
-    <row r="4" ht="14.25" customHeight="1">
+    <row r="1" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:7" ht="14.25" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="2" t="s">
@@ -1577,7 +1538,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" ht="14.25" customHeight="1">
+    <row r="5" spans="1:7" ht="14.25" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1597,7 +1558,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
+    <row r="6" spans="1:7" ht="14.25" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1617,7 +1578,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" ht="14.25" customHeight="1">
+    <row r="7" spans="1:7" ht="14.25" customHeight="1">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -1633,7 +1594,7 @@
       </c>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" ht="14.25" customHeight="1">
+    <row r="8" spans="1:7" ht="14.25" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
@@ -1649,7 +1610,7 @@
       </c>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" ht="14.25" customHeight="1">
+    <row r="9" spans="1:7" ht="14.25" customHeight="1">
       <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
@@ -1670,7 +1631,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" ht="14.25" customHeight="1">
+    <row r="10" spans="1:7" ht="14.25" customHeight="1">
       <c r="A10" s="4" t="s">
         <v>19</v>
       </c>
@@ -1691,7 +1652,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" ht="14.25" customHeight="1">
+    <row r="11" spans="1:7" ht="14.25" customHeight="1">
       <c r="A11" s="4" t="s">
         <v>21</v>
       </c>
@@ -1707,7 +1668,7 @@
       </c>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
+    <row r="12" spans="1:7" ht="14.25" customHeight="1">
       <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
@@ -1723,7 +1684,7 @@
       </c>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" ht="14.25" customHeight="1">
+    <row r="13" spans="1:7" ht="14.25" customHeight="1">
       <c r="A13" s="4" t="s">
         <v>23</v>
       </c>
@@ -1739,7 +1700,7 @@
       </c>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" ht="14.25" customHeight="1">
+    <row r="14" spans="1:7" ht="14.25" customHeight="1">
       <c r="A14" s="4" t="s">
         <v>25</v>
       </c>
@@ -1755,7 +1716,7 @@
       </c>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" ht="14.25" customHeight="1">
+    <row r="15" spans="1:7" ht="14.25" customHeight="1">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -1763,10 +1724,10 @@
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1">
+    <row r="16" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="17" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:7" ht="14.25" customHeight="1">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="9" t="s">
@@ -1776,7 +1737,7 @@
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" ht="14.25" customHeight="1">
+    <row r="20" spans="1:7" ht="14.25" customHeight="1">
       <c r="A20" s="10" t="s">
         <v>28</v>
       </c>
@@ -1796,7 +1757,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" ht="14.25" customHeight="1">
+    <row r="21" spans="1:7" ht="14.25" customHeight="1">
       <c r="A21" s="11" t="s">
         <v>34</v>
       </c>
@@ -1816,7 +1777,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" ht="14.25" customHeight="1">
+    <row r="22" spans="1:7" ht="14.25" customHeight="1">
       <c r="A22" s="11" t="s">
         <v>35</v>
       </c>
@@ -1832,7 +1793,7 @@
       </c>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" ht="14.25" customHeight="1">
+    <row r="23" spans="1:7" ht="14.25" customHeight="1">
       <c r="A23" s="11" t="s">
         <v>36</v>
       </c>
@@ -1848,7 +1809,7 @@
       </c>
       <c r="F23" s="12"/>
     </row>
-    <row r="24" ht="14.25" customHeight="1">
+    <row r="24" spans="1:7" ht="14.25" customHeight="1">
       <c r="A24" s="11" t="s">
         <v>37</v>
       </c>
@@ -1869,7 +1830,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" ht="14.25" customHeight="1">
+    <row r="25" spans="1:7" ht="14.25" customHeight="1">
       <c r="A25" s="11" t="s">
         <v>38</v>
       </c>
@@ -1890,7 +1851,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" ht="14.25" customHeight="1">
+    <row r="26" spans="1:7" ht="14.25" customHeight="1">
       <c r="A26" s="11" t="s">
         <v>39</v>
       </c>
@@ -1906,7 +1867,7 @@
       </c>
       <c r="F26" s="12"/>
     </row>
-    <row r="27" ht="14.25" customHeight="1">
+    <row r="27" spans="1:7" ht="14.25" customHeight="1">
       <c r="A27" s="11" t="s">
         <v>40</v>
       </c>
@@ -1922,7 +1883,7 @@
       </c>
       <c r="F27" s="12"/>
     </row>
-    <row r="28" ht="14.25" customHeight="1">
+    <row r="28" spans="1:7" ht="14.25" customHeight="1">
       <c r="A28" s="11" t="s">
         <v>41</v>
       </c>
@@ -1938,7 +1899,7 @@
       </c>
       <c r="F28" s="12"/>
     </row>
-    <row r="29" ht="14.25" customHeight="1">
+    <row r="29" spans="1:7" ht="14.25" customHeight="1">
       <c r="A29" s="11" t="s">
         <v>42</v>
       </c>
@@ -1954,7 +1915,7 @@
       </c>
       <c r="F29" s="12"/>
     </row>
-    <row r="30" ht="14.25" customHeight="1">
+    <row r="30" spans="1:7" ht="14.25" customHeight="1">
       <c r="A30" s="11" t="s">
         <v>43</v>
       </c>
@@ -1971,7 +1932,7 @@
       <c r="F30" s="12"/>
       <c r="G30" s="13"/>
     </row>
-    <row r="31" ht="14.25" customHeight="1">
+    <row r="31" spans="1:7" ht="14.25" customHeight="1">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -1980,11 +1941,11 @@
       <c r="F31" s="7"/>
       <c r="G31" s="14"/>
     </row>
-    <row r="32" ht="14.25" customHeight="1">
+    <row r="32" spans="1:7" ht="14.25" customHeight="1">
       <c r="G32" s="13"/>
     </row>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1">
+    <row r="33" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="34" spans="1:7" ht="14.25" customHeight="1">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="2" t="s">
@@ -1994,7 +1955,7 @@
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" ht="14.25" customHeight="1">
+    <row r="35" spans="1:7" ht="14.25" customHeight="1">
       <c r="A35" s="3" t="s">
         <v>1</v>
       </c>
@@ -2014,7 +1975,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" ht="14.25" customHeight="1">
+    <row r="36" spans="1:7" ht="14.25" customHeight="1">
       <c r="A36" s="4" t="s">
         <v>46</v>
       </c>
@@ -2034,7 +1995,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" ht="14.25" customHeight="1">
+    <row r="37" spans="1:7" ht="14.25" customHeight="1">
       <c r="A37" s="4" t="s">
         <v>47</v>
       </c>
@@ -2050,7 +2011,7 @@
       </c>
       <c r="F37" s="5"/>
     </row>
-    <row r="38" ht="14.25" customHeight="1">
+    <row r="38" spans="1:7" ht="14.25" customHeight="1">
       <c r="A38" s="4" t="s">
         <v>48</v>
       </c>
@@ -2066,7 +2027,7 @@
       </c>
       <c r="F38" s="5"/>
     </row>
-    <row r="39" ht="14.25" customHeight="1">
+    <row r="39" spans="1:7" ht="14.25" customHeight="1">
       <c r="A39" s="4" t="s">
         <v>49</v>
       </c>
@@ -2082,7 +2043,7 @@
       </c>
       <c r="F39" s="5"/>
     </row>
-    <row r="40" ht="14.25" customHeight="1">
+    <row r="40" spans="1:7" ht="14.25" customHeight="1">
       <c r="A40" s="4" t="s">
         <v>50</v>
       </c>
@@ -2098,7 +2059,7 @@
       </c>
       <c r="F40" s="5"/>
     </row>
-    <row r="41" ht="14.25" customHeight="1">
+    <row r="41" spans="1:7" ht="14.25" customHeight="1">
       <c r="A41" s="4" t="s">
         <v>52</v>
       </c>
@@ -2114,7 +2075,7 @@
       </c>
       <c r="F41" s="5"/>
     </row>
-    <row r="42" ht="14.25" customHeight="1">
+    <row r="42" spans="1:7" ht="14.25" customHeight="1">
       <c r="A42" s="4" t="s">
         <v>55</v>
       </c>
@@ -2130,7 +2091,7 @@
       </c>
       <c r="F42" s="5"/>
     </row>
-    <row r="43" ht="14.25" customHeight="1">
+    <row r="43" spans="1:7" ht="14.25" customHeight="1">
       <c r="A43" s="4" t="s">
         <v>34</v>
       </c>
@@ -2151,7 +2112,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="44" ht="14.25" customHeight="1">
+    <row r="44" spans="1:7" ht="14.25" customHeight="1">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -2159,11 +2120,11 @@
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
     </row>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1">
+    <row r="45" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="49" spans="1:16" ht="14.25" customHeight="1">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="2" t="s">
@@ -2173,13 +2134,13 @@
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="O49" s="15">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="P49" s="15">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="50" ht="14.25" customHeight="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" ht="14.25" customHeight="1">
       <c r="A50" s="3" t="s">
         <v>1</v>
       </c>
@@ -2205,7 +2166,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="51" ht="14.25" customHeight="1">
+    <row r="51" spans="1:16" ht="14.25" customHeight="1">
       <c r="A51" s="4" t="s">
         <v>60</v>
       </c>
@@ -2225,13 +2186,13 @@
         <v>11</v>
       </c>
       <c r="O51" s="15">
-        <v>90.0</v>
+        <v>90</v>
       </c>
       <c r="P51" s="15">
-        <v>36.0</v>
-      </c>
-    </row>
-    <row r="52" ht="14.25" customHeight="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" ht="14.25" customHeight="1">
       <c r="A52" s="4" t="s">
         <v>7</v>
       </c>
@@ -2255,7 +2216,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="53" ht="14.25" customHeight="1">
+    <row r="53" spans="1:16" ht="14.25" customHeight="1">
       <c r="A53" s="4" t="s">
         <v>62</v>
       </c>
@@ -2274,7 +2235,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="54" ht="14.25" customHeight="1">
+    <row r="54" spans="1:16" ht="14.25" customHeight="1">
       <c r="A54" s="4" t="s">
         <v>64</v>
       </c>
@@ -2290,7 +2251,7 @@
       </c>
       <c r="F54" s="5"/>
     </row>
-    <row r="55" ht="14.25" customHeight="1">
+    <row r="55" spans="1:16" ht="14.25" customHeight="1">
       <c r="A55" s="4" t="s">
         <v>65</v>
       </c>
@@ -2306,7 +2267,7 @@
       </c>
       <c r="F55" s="5"/>
     </row>
-    <row r="56" ht="14.25" customHeight="1">
+    <row r="56" spans="1:16" ht="14.25" customHeight="1">
       <c r="A56" s="7"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
@@ -2320,7 +2281,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="57" ht="14.25" customHeight="1">
+    <row r="57" spans="1:16" ht="14.25" customHeight="1">
       <c r="H57" s="15"/>
       <c r="I57" s="15"/>
       <c r="J57" s="15"/>
@@ -2328,18 +2289,18 @@
         <v>67</v>
       </c>
     </row>
-    <row r="58" ht="14.25" customHeight="1">
+    <row r="58" spans="1:16" ht="14.25" customHeight="1">
       <c r="H58" s="15"/>
       <c r="I58" s="15"/>
       <c r="J58" s="15"/>
       <c r="K58" s="15">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" ht="14.25" customHeight="1"/>
+    <row r="60" spans="1:16" ht="14.25" customHeight="1"/>
+    <row r="61" spans="1:16" ht="14.25" customHeight="1"/>
+    <row r="62" spans="1:16" ht="14.25" customHeight="1">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="2" t="s">
@@ -2349,7 +2310,7 @@
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
     </row>
-    <row r="63" ht="14.25" customHeight="1">
+    <row r="63" spans="1:16" ht="14.25" customHeight="1">
       <c r="A63" s="3" t="s">
         <v>1</v>
       </c>
@@ -2369,7 +2330,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" ht="14.25" customHeight="1">
+    <row r="64" spans="1:16" ht="14.25" customHeight="1">
       <c r="A64" s="4" t="s">
         <v>69</v>
       </c>
@@ -2389,7 +2350,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" ht="14.25" customHeight="1">
+    <row r="65" spans="1:22" ht="14.25" customHeight="1">
       <c r="A65" s="4" t="s">
         <v>60</v>
       </c>
@@ -2410,7 +2371,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="66" ht="14.25" customHeight="1">
+    <row r="66" spans="1:22" ht="14.25" customHeight="1">
       <c r="A66" s="4" t="s">
         <v>46</v>
       </c>
@@ -2431,7 +2392,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="67" ht="14.25" customHeight="1">
+    <row r="67" spans="1:22" ht="14.25" customHeight="1">
       <c r="A67" s="4" t="s">
         <v>72</v>
       </c>
@@ -2447,7 +2408,7 @@
       </c>
       <c r="F67" s="5"/>
     </row>
-    <row r="68" ht="14.25" customHeight="1">
+    <row r="68" spans="1:22" ht="14.25" customHeight="1">
       <c r="A68" s="4" t="s">
         <v>73</v>
       </c>
@@ -2464,7 +2425,7 @@
       <c r="F68" s="5"/>
       <c r="J68" s="17"/>
     </row>
-    <row r="69" ht="14.25" customHeight="1">
+    <row r="69" spans="1:22" ht="14.25" customHeight="1">
       <c r="A69" s="4" t="s">
         <v>75</v>
       </c>
@@ -2480,7 +2441,7 @@
       </c>
       <c r="F69" s="5"/>
     </row>
-    <row r="70" ht="14.25" customHeight="1">
+    <row r="70" spans="1:22" ht="14.25" customHeight="1">
       <c r="A70" s="4" t="s">
         <v>76</v>
       </c>
@@ -2496,7 +2457,7 @@
       </c>
       <c r="F70" s="5"/>
     </row>
-    <row r="71" ht="14.25" customHeight="1">
+    <row r="71" spans="1:22" ht="14.25" customHeight="1">
       <c r="A71" s="4" t="s">
         <v>77</v>
       </c>
@@ -2512,7 +2473,7 @@
       </c>
       <c r="F71" s="5"/>
     </row>
-    <row r="72" ht="14.25" customHeight="1">
+    <row r="72" spans="1:22" ht="14.25" customHeight="1">
       <c r="A72" s="4" t="s">
         <v>78</v>
       </c>
@@ -2528,7 +2489,7 @@
       </c>
       <c r="F72" s="5"/>
     </row>
-    <row r="73" ht="14.25" customHeight="1">
+    <row r="73" spans="1:22" ht="14.25" customHeight="1">
       <c r="A73" s="7"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
@@ -2536,16 +2497,16 @@
       <c r="E73" s="7"/>
       <c r="F73" s="7"/>
     </row>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1">
+    <row r="74" spans="1:22" ht="14.25" customHeight="1"/>
+    <row r="75" spans="1:22" ht="14.25" customHeight="1"/>
+    <row r="76" spans="1:22" ht="14.25" customHeight="1">
       <c r="V76" s="18" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1">
+    <row r="77" spans="1:22" ht="14.25" customHeight="1"/>
+    <row r="78" spans="1:22" ht="14.25" customHeight="1"/>
+    <row r="79" spans="1:22" ht="14.25" customHeight="1">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="2" t="s">
@@ -2555,7 +2516,7 @@
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
     </row>
-    <row r="80" ht="14.25" customHeight="1">
+    <row r="80" spans="1:22" ht="14.25" customHeight="1">
       <c r="A80" s="3" t="s">
         <v>1</v>
       </c>
@@ -2575,7 +2536,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" ht="14.25" customHeight="1">
+    <row r="81" spans="1:7" ht="14.25" customHeight="1">
       <c r="A81" s="4" t="s">
         <v>81</v>
       </c>
@@ -2593,7 +2554,7 @@
       </c>
       <c r="F81" s="5"/>
     </row>
-    <row r="82" ht="14.25" customHeight="1">
+    <row r="82" spans="1:7" ht="14.25" customHeight="1">
       <c r="A82" s="4" t="s">
         <v>7</v>
       </c>
@@ -2614,7 +2575,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="83" ht="14.25" customHeight="1">
+    <row r="83" spans="1:7" ht="14.25" customHeight="1">
       <c r="A83" s="4" t="s">
         <v>46</v>
       </c>
@@ -2635,7 +2596,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="84" ht="14.25" customHeight="1">
+    <row r="84" spans="1:7" ht="14.25" customHeight="1">
       <c r="A84" s="4" t="s">
         <v>82</v>
       </c>
@@ -2651,7 +2612,7 @@
       </c>
       <c r="F84" s="5"/>
     </row>
-    <row r="85" ht="14.25" customHeight="1">
+    <row r="85" spans="1:7" ht="14.25" customHeight="1">
       <c r="A85" s="4" t="s">
         <v>83</v>
       </c>
@@ -2667,7 +2628,7 @@
       </c>
       <c r="F85" s="5"/>
     </row>
-    <row r="86" ht="14.25" customHeight="1">
+    <row r="86" spans="1:7" ht="14.25" customHeight="1">
       <c r="A86" s="7"/>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
@@ -2675,11 +2636,11 @@
       <c r="E86" s="7"/>
       <c r="F86" s="7"/>
     </row>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
-    <row r="89" ht="14.25" customHeight="1"/>
-    <row r="90" ht="14.25" customHeight="1"/>
-    <row r="91" ht="14.25" customHeight="1">
+    <row r="87" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="88" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="89" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="90" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="91" spans="1:7" ht="14.25" customHeight="1">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="2" t="s">
@@ -2689,7 +2650,7 @@
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
     </row>
-    <row r="92" ht="14.25" customHeight="1">
+    <row r="92" spans="1:7" ht="14.25" customHeight="1">
       <c r="A92" s="3" t="s">
         <v>1</v>
       </c>
@@ -2709,7 +2670,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="93" ht="14.25" customHeight="1">
+    <row r="93" spans="1:7" ht="14.25" customHeight="1">
       <c r="A93" s="4" t="s">
         <v>86</v>
       </c>
@@ -2729,7 +2690,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="94" ht="14.25" customHeight="1">
+    <row r="94" spans="1:7" ht="14.25" customHeight="1">
       <c r="A94" s="4" t="s">
         <v>7</v>
       </c>
@@ -2747,7 +2708,7 @@
       </c>
       <c r="F94" s="5"/>
     </row>
-    <row r="95" ht="14.25" customHeight="1">
+    <row r="95" spans="1:7" ht="14.25" customHeight="1">
       <c r="A95" s="4" t="s">
         <v>34</v>
       </c>
@@ -2768,7 +2729,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="96" ht="14.25" customHeight="1">
+    <row r="96" spans="1:7" ht="14.25" customHeight="1">
       <c r="A96" s="4" t="s">
         <v>46</v>
       </c>
@@ -2789,7 +2750,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="97" ht="14.25" customHeight="1">
+    <row r="97" spans="1:7" ht="14.25" customHeight="1">
       <c r="A97" s="4" t="s">
         <v>87</v>
       </c>
@@ -2808,7 +2769,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="98" ht="14.25" customHeight="1">
+    <row r="98" spans="1:7" ht="14.25" customHeight="1">
       <c r="A98" s="4" t="s">
         <v>89</v>
       </c>
@@ -2824,7 +2785,7 @@
       </c>
       <c r="F98" s="5"/>
     </row>
-    <row r="99" ht="14.25" customHeight="1">
+    <row r="99" spans="1:7" ht="14.25" customHeight="1">
       <c r="A99" s="7"/>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
@@ -2832,19 +2793,19 @@
       <c r="E99" s="7"/>
       <c r="F99" s="7"/>
     </row>
-    <row r="100" ht="14.25" customHeight="1"/>
-    <row r="101" ht="14.25" customHeight="1"/>
-    <row r="102" ht="14.25" customHeight="1"/>
-    <row r="103" ht="14.25" customHeight="1"/>
-    <row r="104" ht="14.25" customHeight="1"/>
-    <row r="105" ht="14.25" customHeight="1"/>
-    <row r="106" ht="14.25" customHeight="1"/>
-    <row r="107" ht="14.25" customHeight="1"/>
-    <row r="108" ht="14.25" customHeight="1"/>
-    <row r="109" ht="14.25" customHeight="1"/>
-    <row r="110" ht="14.25" customHeight="1"/>
-    <row r="111" ht="14.25" customHeight="1"/>
-    <row r="112" ht="14.25" customHeight="1"/>
+    <row r="100" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="101" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="102" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="103" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="104" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="105" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="106" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="107" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="108" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="109" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="110" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="111" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="112" spans="1:7" ht="14.25" customHeight="1"/>
     <row r="113" ht="14.25" customHeight="1"/>
     <row r="114" ht="14.25" customHeight="1"/>
     <row r="115" ht="14.25" customHeight="1"/>
@@ -3680,36 +3641,37 @@
     <row r="945" ht="14.25" customHeight="1"/>
     <row r="946" ht="14.25" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A3:Y74"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="H76" sqref="H76"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="15.0"/>
-    <col customWidth="1" min="2" max="2" width="19.57"/>
-    <col customWidth="1" min="3" max="3" width="22.57"/>
-    <col customWidth="1" min="4" max="4" width="22.29"/>
-    <col customWidth="1" min="5" max="5" width="21.86"/>
-    <col customWidth="1" min="6" max="6" width="21.57"/>
-    <col customWidth="1" min="7" max="7" width="17.29"/>
-    <col customWidth="1" min="8" max="8" width="29.86"/>
-    <col customWidth="1" min="9" max="9" width="53.29"/>
-    <col customWidth="1" min="10" max="10" width="27.29"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="29.85546875" customWidth="1"/>
+    <col min="9" max="9" width="53.28515625" customWidth="1"/>
+    <col min="10" max="10" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3">
+    <row r="3" spans="1:25">
       <c r="A3" s="19" t="s">
         <v>90</v>
       </c>
@@ -3724,7 +3686,7 @@
       <c r="H3" s="19"/>
       <c r="I3" s="19"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:25">
       <c r="A4" s="20" t="s">
         <v>7</v>
       </c>
@@ -3743,19 +3705,19 @@
       <c r="F4" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="21" t="s">
-        <v>93</v>
+      <c r="G4" s="75" t="s">
+        <v>275</v>
       </c>
       <c r="H4" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="20" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="I4" s="76" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25">
       <c r="A5" s="22">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="B5" s="22" t="s">
         <v>95</v>
@@ -3764,7 +3726,7 @@
         <v>96</v>
       </c>
       <c r="D5" s="22">
-        <v>7.41258963E9</v>
+        <v>7412589630</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>97</v>
@@ -3779,7 +3741,7 @@
         <v>99</v>
       </c>
       <c r="I5" s="22">
-        <v>411002.0</v>
+        <v>411002</v>
       </c>
       <c r="J5" s="23"/>
       <c r="K5" s="23"/>
@@ -3798,9 +3760,9 @@
       <c r="X5" s="23"/>
       <c r="Y5" s="23"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:25">
       <c r="A6" s="22">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>100</v>
@@ -3809,7 +3771,7 @@
         <v>101</v>
       </c>
       <c r="D6" s="22">
-        <v>8.56598529E9</v>
+        <v>8565985290</v>
       </c>
       <c r="E6" s="22" t="s">
         <v>102</v>
@@ -3824,12 +3786,12 @@
         <v>104</v>
       </c>
       <c r="I6" s="22">
-        <v>444901.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>444901</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25">
       <c r="A7" s="22">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="B7" s="22" t="s">
         <v>105</v>
@@ -3838,7 +3800,7 @@
         <v>106</v>
       </c>
       <c r="D7" s="22">
-        <v>9.71938095E9</v>
+        <v>9719380950</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>107</v>
@@ -3853,12 +3815,12 @@
         <v>109</v>
       </c>
       <c r="I7" s="22">
-        <v>413510.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>413510</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25">
       <c r="A8" s="22">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="B8" s="22" t="s">
         <v>110</v>
@@ -3867,7 +3829,7 @@
         <v>111</v>
       </c>
       <c r="D8" s="22">
-        <v>9.887277661E9</v>
+        <v>9887277661</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>112</v>
@@ -3882,12 +3844,12 @@
         <v>114</v>
       </c>
       <c r="I8" s="22">
-        <v>410005.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>410005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25">
       <c r="A9" s="22">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="B9" s="22" t="s">
         <v>115</v>
@@ -3896,7 +3858,7 @@
         <v>116</v>
       </c>
       <c r="D9" s="22">
-        <v>9.902617227E9</v>
+        <v>9902617227</v>
       </c>
       <c r="E9" s="22" t="s">
         <v>117</v>
@@ -3911,10 +3873,10 @@
         <v>119</v>
       </c>
       <c r="I9" s="22">
-        <v>400030.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>400030</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25">
       <c r="A11" s="24"/>
       <c r="B11" s="24"/>
       <c r="C11" s="25" t="s">
@@ -3923,7 +3885,7 @@
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:25">
       <c r="A12" s="26" t="s">
         <v>60</v>
       </c>
@@ -3940,92 +3902,92 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:25">
       <c r="A13" s="22">
-        <v>101.0</v>
+        <v>101</v>
       </c>
       <c r="B13" s="22">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="C13" s="29">
-        <v>51000.0</v>
+        <v>51000</v>
       </c>
       <c r="D13" s="29">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="30">
-        <v>44896.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>44896</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25">
       <c r="A14" s="22">
-        <v>102.0</v>
+        <v>102</v>
       </c>
       <c r="B14" s="22">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="C14" s="29">
-        <v>22000.0</v>
+        <v>22000</v>
       </c>
       <c r="D14" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="22" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:25">
       <c r="A15" s="22">
-        <v>103.0</v>
+        <v>103</v>
       </c>
       <c r="B15" s="22">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="C15" s="22">
-        <v>8000.0</v>
+        <v>8000</v>
       </c>
       <c r="D15" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="22" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:25">
       <c r="A16" s="22">
-        <v>104.0</v>
+        <v>104</v>
       </c>
       <c r="B16" s="22">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="C16" s="22">
-        <v>6200.0</v>
+        <v>6200</v>
       </c>
       <c r="D16" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="22" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:10">
       <c r="A17" s="22">
-        <v>105.0</v>
+        <v>105</v>
       </c>
       <c r="B17" s="22">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="C17" s="22">
-        <v>6600.0</v>
+        <v>6600</v>
       </c>
       <c r="D17" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="22" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:10">
       <c r="A19" s="24"/>
       <c r="B19" s="24"/>
       <c r="C19" s="24"/>
@@ -4038,7 +4000,7 @@
       <c r="H19" s="24"/>
       <c r="I19" s="24"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:10">
       <c r="A20" s="32" t="s">
         <v>69</v>
       </c>
@@ -4067,15 +4029,15 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:10">
       <c r="A21" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B21" s="22">
-        <v>101.0</v>
+        <v>101</v>
       </c>
       <c r="C21" s="22">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="D21" s="22" t="s">
         <v>125</v>
@@ -4090,21 +4052,21 @@
         <v>126</v>
       </c>
       <c r="H21" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="22" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:10">
       <c r="A22" s="22">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B22" s="22">
-        <v>101.0</v>
+        <v>101</v>
       </c>
       <c r="C22" s="22">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="D22" s="22" t="s">
         <v>125</v>
@@ -4119,21 +4081,21 @@
         <v>126</v>
       </c>
       <c r="H22" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="22" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:10">
       <c r="A23" s="22">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B23" s="22">
-        <v>101.0</v>
+        <v>101</v>
       </c>
       <c r="C23" s="22">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="D23" s="22" t="s">
         <v>125</v>
@@ -4148,21 +4110,21 @@
         <v>126</v>
       </c>
       <c r="H23" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="I23" s="22" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:10">
       <c r="A24" s="22">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B24" s="22">
-        <v>102.0</v>
+        <v>102</v>
       </c>
       <c r="C24" s="22">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="D24" s="22" t="s">
         <v>128</v>
@@ -4177,21 +4139,21 @@
         <v>130</v>
       </c>
       <c r="H24" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="I24" s="22" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:10">
       <c r="A25" s="22">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B25" s="22">
-        <v>102.0</v>
+        <v>102</v>
       </c>
       <c r="C25" s="22">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="D25" s="22" t="s">
         <v>128</v>
@@ -4206,21 +4168,21 @@
         <v>129</v>
       </c>
       <c r="H25" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="I25" s="22" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:10">
       <c r="A26" s="22">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B26" s="22">
-        <v>103.0</v>
+        <v>103</v>
       </c>
       <c r="C26" s="22">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="D26" s="22" t="s">
         <v>132</v>
@@ -4235,21 +4197,21 @@
         <v>135</v>
       </c>
       <c r="H26" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="I26" s="22" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:10">
       <c r="A27" s="22">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B27" s="22">
-        <v>104.0</v>
+        <v>104</v>
       </c>
       <c r="C27" s="22">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="D27" s="22" t="s">
         <v>136</v>
@@ -4264,21 +4226,21 @@
         <v>137</v>
       </c>
       <c r="H27" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="I27" s="22" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:10">
       <c r="A28" s="22">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B28" s="22">
-        <v>104.0</v>
+        <v>104</v>
       </c>
       <c r="C28" s="22">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="D28" s="22" t="s">
         <v>136</v>
@@ -4293,21 +4255,21 @@
         <v>139</v>
       </c>
       <c r="H28" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="I28" s="22" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:10">
       <c r="A29" s="22">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B29" s="22">
-        <v>105.0</v>
+        <v>105</v>
       </c>
       <c r="C29" s="22">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="D29" s="22" t="s">
         <v>140</v>
@@ -4322,13 +4284,13 @@
         <v>142</v>
       </c>
       <c r="H29" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="I29" s="22" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:10">
       <c r="A31" s="24"/>
       <c r="B31" s="24"/>
       <c r="C31" s="24"/>
@@ -4342,7 +4304,7 @@
       <c r="I31" s="24"/>
       <c r="J31" s="24"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:10">
       <c r="A32" s="33" t="s">
         <v>34</v>
       </c>
@@ -4374,9 +4336,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:25">
       <c r="A33" s="34">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B33" s="35" t="s">
         <v>143</v>
@@ -4385,7 +4347,7 @@
         <v>144</v>
       </c>
       <c r="D33" s="36">
-        <v>9.87456321E9</v>
+        <v>9874563210</v>
       </c>
       <c r="E33" s="35" t="s">
         <v>145</v>
@@ -4403,15 +4365,15 @@
         <v>148</v>
       </c>
       <c r="J33" s="34">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="Y33" s="15">
-        <v>91.0</v>
-      </c>
-    </row>
-    <row r="34">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25">
       <c r="A34" s="34">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B34" s="35" t="s">
         <v>149</v>
@@ -4420,7 +4382,7 @@
         <v>150</v>
       </c>
       <c r="D34" s="36">
-        <v>9.874563212E9</v>
+        <v>9874563212</v>
       </c>
       <c r="E34" s="35" t="s">
         <v>151</v>
@@ -4438,15 +4400,15 @@
         <v>154</v>
       </c>
       <c r="J34" s="34">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="Y34" s="15">
-        <v>92.0</v>
-      </c>
-    </row>
-    <row r="35">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25">
       <c r="A35" s="34">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B35" s="35" t="s">
         <v>155</v>
@@ -4455,7 +4417,7 @@
         <v>156</v>
       </c>
       <c r="D35" s="36">
-        <v>9.874563215E9</v>
+        <v>9874563215</v>
       </c>
       <c r="E35" s="35" t="s">
         <v>157</v>
@@ -4473,15 +4435,15 @@
         <v>160</v>
       </c>
       <c r="J35" s="34">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="Y35" s="15">
-        <v>96.0</v>
-      </c>
-    </row>
-    <row r="36">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25">
       <c r="A36" s="34">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B36" s="35" t="s">
         <v>161</v>
@@ -4490,7 +4452,7 @@
         <v>162</v>
       </c>
       <c r="D36" s="36">
-        <v>9.874563218E9</v>
+        <v>9874563218</v>
       </c>
       <c r="E36" s="35" t="s">
         <v>163</v>
@@ -4508,15 +4470,15 @@
         <v>166</v>
       </c>
       <c r="J36" s="34">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="Y36" s="15">
-        <v>97.0</v>
-      </c>
-    </row>
-    <row r="37">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25">
       <c r="A37" s="34">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B37" s="35" t="s">
         <v>167</v>
@@ -4525,7 +4487,7 @@
         <v>168</v>
       </c>
       <c r="D37" s="36">
-        <v>9.87456322E9</v>
+        <v>9874563220</v>
       </c>
       <c r="E37" s="35" t="s">
         <v>169</v>
@@ -4543,13 +4505,13 @@
         <v>172</v>
       </c>
       <c r="J37" s="34">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="Y37" s="15">
-        <v>101.0</v>
-      </c>
-    </row>
-    <row r="39">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25">
       <c r="A39" s="37"/>
       <c r="B39" s="38"/>
       <c r="C39" s="39"/>
@@ -4567,7 +4529,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:25">
       <c r="A40" s="33" t="s">
         <v>46</v>
       </c>
@@ -4599,9 +4561,9 @@
         <v>177</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:25">
       <c r="A41" s="42">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="B41" s="29" t="s">
         <v>178</v>
@@ -4613,24 +4575,24 @@
         <v>180</v>
       </c>
       <c r="E41" s="42">
-        <v>1500.0</v>
+        <v>1500</v>
       </c>
       <c r="F41" s="42" t="s">
         <v>181</v>
       </c>
       <c r="G41" s="42">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H41" s="42">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="Y41" s="15" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:25">
       <c r="A42" s="42">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="B42" s="42" t="s">
         <v>183</v>
@@ -4642,24 +4604,24 @@
         <v>180</v>
       </c>
       <c r="E42" s="42">
-        <v>2000.0</v>
+        <v>2000</v>
       </c>
       <c r="F42" s="42" t="s">
         <v>185</v>
       </c>
       <c r="G42" s="42">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H42" s="42">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="Y42" s="15" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:25">
       <c r="A43" s="22">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="B43" s="22" t="s">
         <v>187</v>
@@ -4671,24 +4633,24 @@
         <v>180</v>
       </c>
       <c r="E43" s="22">
-        <v>5000.0</v>
+        <v>5000</v>
       </c>
       <c r="F43" s="22" t="s">
         <v>189</v>
       </c>
       <c r="G43" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H43" s="22">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="Y43" s="15" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:25">
       <c r="A44" s="42">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="B44" s="42" t="s">
         <v>191</v>
@@ -4700,24 +4662,24 @@
         <v>193</v>
       </c>
       <c r="E44" s="42">
-        <v>1000.0</v>
+        <v>1000</v>
       </c>
       <c r="F44" s="42" t="s">
         <v>194</v>
       </c>
       <c r="G44" s="42">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H44" s="42">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="Y44" s="15" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:25">
       <c r="A45" s="42">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="B45" s="42" t="s">
         <v>196</v>
@@ -4729,24 +4691,24 @@
         <v>180</v>
       </c>
       <c r="E45" s="42">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="F45" s="42" t="s">
         <v>198</v>
       </c>
       <c r="G45" s="42">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H45" s="42">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="Y45" s="15" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:25">
       <c r="A46" s="42">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="B46" s="42" t="s">
         <v>200</v>
@@ -4758,21 +4720,21 @@
         <v>193</v>
       </c>
       <c r="E46" s="42">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="F46" s="42" t="s">
         <v>202</v>
       </c>
       <c r="G46" s="42">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H46" s="42">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25">
       <c r="A47" s="42">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="B47" s="42" t="s">
         <v>203</v>
@@ -4784,19 +4746,19 @@
         <v>193</v>
       </c>
       <c r="E47" s="42">
-        <v>600.0</v>
+        <v>600</v>
       </c>
       <c r="F47" s="42" t="s">
         <v>205</v>
       </c>
       <c r="G47" s="42">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H47" s="42">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" s="43"/>
       <c r="B49" s="43"/>
       <c r="C49" s="44"/>
@@ -4806,7 +4768,7 @@
       <c r="E49" s="43"/>
       <c r="F49" s="45"/>
     </row>
-    <row r="50">
+    <row r="50" spans="1:6">
       <c r="A50" s="32" t="s">
         <v>207</v>
       </c>
@@ -4826,13 +4788,13 @@
         <v>209</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:6">
       <c r="A51" s="22">
-        <v>91.0</v>
+        <v>91</v>
       </c>
       <c r="B51" s="22"/>
       <c r="C51" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D51" s="49"/>
       <c r="E51" s="22" t="s">
@@ -4842,13 +4804,13 @@
         <v>211</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:6">
       <c r="A52" s="22">
-        <v>92.0</v>
+        <v>92</v>
       </c>
       <c r="B52" s="22"/>
       <c r="C52" s="22">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D52" s="49"/>
       <c r="E52" s="22" t="s">
@@ -4858,13 +4820,13 @@
         <v>211</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:6">
       <c r="A53" s="22">
-        <v>93.0</v>
+        <v>93</v>
       </c>
       <c r="B53" s="22"/>
       <c r="C53" s="22">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="D53" s="49"/>
       <c r="E53" s="22" t="s">
@@ -4874,13 +4836,13 @@
         <v>211</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:6">
       <c r="A54" s="22">
-        <v>94.0</v>
+        <v>94</v>
       </c>
       <c r="B54" s="22"/>
       <c r="C54" s="22">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="D54" s="49"/>
       <c r="E54" s="22" t="s">
@@ -4890,13 +4852,13 @@
         <v>211</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:6">
       <c r="A55" s="22">
-        <v>95.0</v>
+        <v>95</v>
       </c>
       <c r="B55" s="22"/>
       <c r="C55" s="22">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="D55" s="49"/>
       <c r="E55" s="22" t="s">
@@ -4906,14 +4868,14 @@
         <v>211</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:6">
       <c r="A56" s="22">
-        <v>96.0</v>
+        <v>96</v>
       </c>
       <c r="B56" s="22"/>
       <c r="C56" s="22"/>
       <c r="D56" s="22">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="E56" s="22" t="s">
         <v>216</v>
@@ -4922,14 +4884,14 @@
         <v>217</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:6">
       <c r="A57" s="22">
-        <v>97.0</v>
+        <v>97</v>
       </c>
       <c r="B57" s="22"/>
       <c r="C57" s="22"/>
       <c r="D57" s="22">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="E57" s="22" t="s">
         <v>218</v>
@@ -4938,14 +4900,14 @@
         <v>217</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:6">
       <c r="A58" s="22">
-        <v>98.0</v>
+        <v>98</v>
       </c>
       <c r="B58" s="22"/>
       <c r="C58" s="22"/>
       <c r="D58" s="22">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="E58" s="22" t="s">
         <v>219</v>
@@ -4954,30 +4916,30 @@
         <v>217</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:6">
       <c r="A59" s="22">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="B59" s="22"/>
       <c r="C59" s="22"/>
       <c r="D59" s="22">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="E59" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="F59" s="50" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="60">
+      <c r="F59" s="77" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" s="22">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="B60" s="22"/>
       <c r="C60" s="22"/>
       <c r="D60" s="22">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="E60" s="22" t="s">
         <v>221</v>
@@ -4986,14 +4948,14 @@
         <v>217</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:6">
       <c r="A61" s="22">
-        <v>101.0</v>
+        <v>101</v>
       </c>
       <c r="B61" s="22"/>
       <c r="C61" s="22"/>
       <c r="D61" s="22">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="E61" s="22" t="s">
         <v>222</v>
@@ -5002,14 +4964,14 @@
         <v>217</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:6">
       <c r="A62" s="22">
-        <v>102.0</v>
+        <v>102</v>
       </c>
       <c r="B62" s="22"/>
       <c r="C62" s="22"/>
       <c r="D62" s="22">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="E62" s="22" t="s">
         <v>223</v>
@@ -5018,28 +4980,28 @@
         <v>217</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:6">
       <c r="A63" s="22">
-        <v>103.0</v>
+        <v>103</v>
       </c>
       <c r="B63" s="22"/>
       <c r="C63" s="22"/>
       <c r="D63" s="22">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="E63" s="22" t="s">
         <v>224</v>
       </c>
-      <c r="F63" s="50" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="64">
+      <c r="F63" s="77" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" s="22">
-        <v>104.0</v>
+        <v>104</v>
       </c>
       <c r="B64" s="22">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="C64" s="49"/>
       <c r="D64" s="49"/>
@@ -5050,12 +5012,12 @@
         <v>226</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:6">
       <c r="A65" s="22">
-        <v>104.0</v>
+        <v>104</v>
       </c>
       <c r="B65" s="22">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="C65" s="22"/>
       <c r="D65" s="49"/>
@@ -5066,12 +5028,12 @@
         <v>226</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:6">
       <c r="A66" s="22">
-        <v>105.0</v>
+        <v>105</v>
       </c>
       <c r="B66" s="22">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="C66" s="22"/>
       <c r="D66" s="49"/>
@@ -5082,7 +5044,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:6">
       <c r="A68" s="43"/>
       <c r="B68" s="43"/>
       <c r="C68" s="44" t="s">
@@ -5091,7 +5053,7 @@
       <c r="D68" s="43"/>
       <c r="E68" s="43"/>
     </row>
-    <row r="69">
+    <row r="69" spans="1:6">
       <c r="A69" s="47" t="s">
         <v>230</v>
       </c>
@@ -5108,140 +5070,147 @@
         <v>234</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:6">
       <c r="A70" s="22">
-        <v>41.0</v>
+        <v>41</v>
       </c>
       <c r="B70" s="22">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="C70" s="51">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="D70" s="22">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E70" s="51" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:6">
       <c r="A71" s="22">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="B71" s="22">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="C71" s="51">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="D71" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E71" s="51" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:6">
       <c r="A72" s="22">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="B72" s="22">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="C72" s="51">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="D72" s="22">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="E72" s="51" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:6">
       <c r="A73" s="22">
-        <v>44.0</v>
+        <v>44</v>
       </c>
       <c r="B73" s="22">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="C73" s="51">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="D73" s="22">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E73" s="51" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:6">
       <c r="A74" s="22">
-        <v>45.0</v>
+        <v>45</v>
       </c>
       <c r="B74" s="22">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="C74" s="51">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="D74" s="22">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E74" s="51" t="s">
         <v>235</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A2:S105"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="17.0"/>
-    <col customWidth="1" min="3" max="3" width="19.0"/>
-    <col customWidth="1" min="4" max="4" width="21.0"/>
-    <col customWidth="1" min="5" max="5" width="19.43"/>
-    <col customWidth="1" min="6" max="6" width="21.57"/>
-    <col customWidth="1" min="7" max="7" width="28.0"/>
-    <col customWidth="1" min="8" max="8" width="22.43"/>
-    <col customWidth="1" min="9" max="9" width="24.0"/>
-    <col customWidth="1" min="10" max="10" width="19.29"/>
-    <col customWidth="1" min="13" max="13" width="19.0"/>
-    <col customWidth="1" min="15" max="15" width="18.14"/>
-    <col customWidth="1" min="18" max="18" width="17.14"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" customWidth="1"/>
+    <col min="7" max="7" width="28" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" customWidth="1"/>
+    <col min="9" max="9" width="24" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" customWidth="1"/>
+    <col min="13" max="13" width="19" customWidth="1"/>
+    <col min="15" max="15" width="18.140625" customWidth="1"/>
+    <col min="18" max="18" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="1:19">
       <c r="L2" s="15" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:19">
       <c r="A3" s="52"/>
       <c r="B3" s="52"/>
       <c r="C3" s="52"/>
@@ -5263,7 +5232,7 @@
       <c r="Q3" s="52"/>
       <c r="R3" s="52"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:19">
       <c r="A4" s="33" t="s">
         <v>34</v>
       </c>
@@ -5314,9 +5283,9 @@
       </c>
       <c r="S4" s="56"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:19">
       <c r="A5" s="57">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B5" s="58" t="s">
         <v>143</v>
@@ -5325,7 +5294,7 @@
         <v>144</v>
       </c>
       <c r="D5" s="59">
-        <v>9.87456321E9</v>
+        <v>9874563210</v>
       </c>
       <c r="E5" s="58" t="s">
         <v>145</v>
@@ -5343,7 +5312,7 @@
         <v>148</v>
       </c>
       <c r="J5" s="57">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M5" s="60" t="s">
         <v>34</v>
@@ -5365,9 +5334,9 @@
       </c>
       <c r="S5" s="62"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:19">
       <c r="A6" s="57">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B6" s="58" t="s">
         <v>149</v>
@@ -5376,7 +5345,7 @@
         <v>150</v>
       </c>
       <c r="D6" s="59">
-        <v>9.874563212E9</v>
+        <v>9874563212</v>
       </c>
       <c r="E6" s="58" t="s">
         <v>151</v>
@@ -5394,7 +5363,7 @@
         <v>154</v>
       </c>
       <c r="J6" s="57">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M6" s="60" t="s">
         <v>35</v>
@@ -5412,9 +5381,9 @@
       <c r="R6" s="63"/>
       <c r="S6" s="63"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:19">
       <c r="A7" s="57">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B7" s="58" t="s">
         <v>155</v>
@@ -5423,7 +5392,7 @@
         <v>156</v>
       </c>
       <c r="D7" s="59">
-        <v>9.874563215E9</v>
+        <v>9874563215</v>
       </c>
       <c r="E7" s="58" t="s">
         <v>157</v>
@@ -5441,7 +5410,7 @@
         <v>160</v>
       </c>
       <c r="J7" s="57">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M7" s="60" t="s">
         <v>36</v>
@@ -5459,9 +5428,9 @@
       <c r="R7" s="63"/>
       <c r="S7" s="63"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:19">
       <c r="A8" s="57">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B8" s="58" t="s">
         <v>161</v>
@@ -5470,7 +5439,7 @@
         <v>162</v>
       </c>
       <c r="D8" s="59">
-        <v>9.874563218E9</v>
+        <v>9874563218</v>
       </c>
       <c r="E8" s="58" t="s">
         <v>163</v>
@@ -5488,7 +5457,7 @@
         <v>166</v>
       </c>
       <c r="J8" s="57">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M8" s="60" t="s">
         <v>37</v>
@@ -5506,9 +5475,9 @@
       <c r="R8" s="63"/>
       <c r="S8" s="63"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:19">
       <c r="A9" s="57">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B9" s="58" t="s">
         <v>167</v>
@@ -5517,7 +5486,7 @@
         <v>168</v>
       </c>
       <c r="D9" s="59">
-        <v>9.87456322E9</v>
+        <v>9874563220</v>
       </c>
       <c r="E9" s="58" t="s">
         <v>169</v>
@@ -5535,7 +5504,7 @@
         <v>172</v>
       </c>
       <c r="J9" s="57">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M9" s="60" t="s">
         <v>38</v>
@@ -5555,7 +5524,7 @@
       <c r="R9" s="63"/>
       <c r="S9" s="63"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:19">
       <c r="M10" s="60" t="s">
         <v>39</v>
       </c>
@@ -5572,7 +5541,7 @@
       <c r="R10" s="63"/>
       <c r="S10" s="63"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:19">
       <c r="M11" s="60" t="s">
         <v>40</v>
       </c>
@@ -5589,7 +5558,7 @@
       <c r="R11" s="63"/>
       <c r="S11" s="63"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:19">
       <c r="M12" s="60" t="s">
         <v>41</v>
       </c>
@@ -5606,7 +5575,7 @@
       <c r="R12" s="63"/>
       <c r="S12" s="63"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:19">
       <c r="M13" s="60" t="s">
         <v>42</v>
       </c>
@@ -5623,7 +5592,7 @@
       <c r="R13" s="63"/>
       <c r="S13" s="63"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:19">
       <c r="M14" s="64" t="s">
         <v>247</v>
       </c>
@@ -5640,7 +5609,7 @@
       <c r="R14" s="65"/>
       <c r="S14" s="65"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:19">
       <c r="M15" s="60" t="s">
         <v>43</v>
       </c>
@@ -5657,7 +5626,7 @@
       <c r="R15" s="63"/>
       <c r="S15" s="63"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:19">
       <c r="M16" s="56"/>
       <c r="N16" s="56"/>
       <c r="O16" s="56"/>
@@ -5665,7 +5634,7 @@
       <c r="Q16" s="56"/>
       <c r="R16" s="56"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:18">
       <c r="A20" s="37"/>
       <c r="B20" s="38"/>
       <c r="C20" s="39"/>
@@ -5678,7 +5647,7 @@
       <c r="H20" s="38"/>
       <c r="J20" s="56"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:18">
       <c r="A21" s="33" t="s">
         <v>46</v>
       </c>
@@ -5713,9 +5682,9 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:18">
       <c r="A22" s="42">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="B22" s="29" t="s">
         <v>178</v>
@@ -5727,16 +5696,16 @@
         <v>180</v>
       </c>
       <c r="E22" s="42">
-        <v>1500.0</v>
+        <v>1500</v>
       </c>
       <c r="F22" s="42" t="s">
         <v>181</v>
       </c>
       <c r="G22" s="42">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="42">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="J22" s="56"/>
       <c r="M22" s="3" t="s">
@@ -5758,9 +5727,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:18">
       <c r="A23" s="42">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="B23" s="42" t="s">
         <v>183</v>
@@ -5772,16 +5741,16 @@
         <v>180</v>
       </c>
       <c r="E23" s="42">
-        <v>2000.0</v>
+        <v>2000</v>
       </c>
       <c r="F23" s="42" t="s">
         <v>185</v>
       </c>
       <c r="G23" s="42">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H23" s="42">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="J23" s="56"/>
       <c r="M23" s="5" t="s">
@@ -5803,9 +5772,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:18">
       <c r="A24" s="22">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="B24" s="22" t="s">
         <v>187</v>
@@ -5817,16 +5786,16 @@
         <v>180</v>
       </c>
       <c r="E24" s="22">
-        <v>5000.0</v>
+        <v>5000</v>
       </c>
       <c r="F24" s="22" t="s">
         <v>189</v>
       </c>
       <c r="G24" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H24" s="22">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="J24" s="56"/>
       <c r="M24" s="5" t="s">
@@ -5844,9 +5813,9 @@
       </c>
       <c r="R24" s="5"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:18">
       <c r="A25" s="42">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="B25" s="42" t="s">
         <v>191</v>
@@ -5858,16 +5827,16 @@
         <v>193</v>
       </c>
       <c r="E25" s="42">
-        <v>1000.0</v>
+        <v>1000</v>
       </c>
       <c r="F25" s="42" t="s">
         <v>194</v>
       </c>
       <c r="G25" s="42">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H25" s="42">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="J25" s="56"/>
       <c r="M25" s="5" t="s">
@@ -5885,9 +5854,9 @@
       </c>
       <c r="R25" s="5"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:18">
       <c r="A26" s="42">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="B26" s="42" t="s">
         <v>196</v>
@@ -5899,16 +5868,16 @@
         <v>180</v>
       </c>
       <c r="E26" s="42">
-        <v>3000.0</v>
+        <v>3000</v>
       </c>
       <c r="F26" s="42" t="s">
         <v>198</v>
       </c>
       <c r="G26" s="42">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H26" s="42">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="J26" s="56"/>
       <c r="M26" s="5" t="s">
@@ -5926,9 +5895,9 @@
       </c>
       <c r="R26" s="5"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:18">
       <c r="A27" s="42">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="B27" s="42" t="s">
         <v>200</v>
@@ -5940,16 +5909,16 @@
         <v>193</v>
       </c>
       <c r="E27" s="42">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="F27" s="42" t="s">
         <v>202</v>
       </c>
       <c r="G27" s="42">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H27" s="42">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="J27" s="56"/>
       <c r="M27" s="5" t="s">
@@ -5967,9 +5936,9 @@
       </c>
       <c r="R27" s="5"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:18">
       <c r="A28" s="42">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="B28" s="42" t="s">
         <v>203</v>
@@ -5981,16 +5950,16 @@
         <v>193</v>
       </c>
       <c r="E28" s="42">
-        <v>600.0</v>
+        <v>600</v>
       </c>
       <c r="F28" s="42" t="s">
         <v>205</v>
       </c>
       <c r="G28" s="42">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H28" s="42">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="J28" s="56"/>
       <c r="M28" s="5" t="s">
@@ -6008,7 +5977,7 @@
       </c>
       <c r="R28" s="5"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:18">
       <c r="B29" s="67"/>
       <c r="C29" s="68"/>
       <c r="D29" s="68"/>
@@ -6033,7 +6002,7 @@
       </c>
       <c r="R29" s="5"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:18">
       <c r="M30" s="5" t="s">
         <v>256</v>
       </c>
@@ -6051,7 +6020,7 @@
       </c>
       <c r="R30" s="5"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:18">
       <c r="A31" s="42"/>
       <c r="M31" s="7"/>
       <c r="N31" s="7"/>
@@ -6060,7 +6029,7 @@
       <c r="Q31" s="7"/>
       <c r="R31" s="7"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:18">
       <c r="A35" s="43"/>
       <c r="B35" s="43"/>
       <c r="C35" s="44" t="s">
@@ -6078,7 +6047,7 @@
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:18">
       <c r="A36" s="32" t="s">
         <v>207</v>
       </c>
@@ -6113,15 +6082,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:18">
       <c r="A37" s="51">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="B37" s="51" t="s">
         <v>260</v>
       </c>
       <c r="C37" s="51">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D37" s="51" t="s">
         <v>261</v>
@@ -6148,15 +6117,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:18">
       <c r="A38" s="51">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="B38" s="51" t="s">
         <v>260</v>
       </c>
       <c r="C38" s="51">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D38" s="51" t="s">
         <v>263</v>
@@ -6179,15 +6148,15 @@
       </c>
       <c r="R38" s="5"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:18">
       <c r="A39" s="51">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="B39" s="51" t="s">
         <v>217</v>
       </c>
       <c r="C39" s="51">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="D39" s="51" t="s">
         <v>223</v>
@@ -6210,15 +6179,15 @@
       </c>
       <c r="R39" s="5"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:18">
       <c r="A40" s="51">
-        <v>34.0</v>
+        <v>34</v>
       </c>
       <c r="B40" s="51" t="s">
         <v>217</v>
       </c>
       <c r="C40" s="51">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="D40" s="51" t="s">
         <v>196</v>
@@ -6241,15 +6210,15 @@
       </c>
       <c r="R40" s="5"/>
     </row>
-    <row r="41">
+    <row r="41" spans="1:18">
       <c r="A41" s="51">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="B41" s="51" t="s">
         <v>266</v>
       </c>
       <c r="C41" s="51">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="D41" s="51" t="s">
         <v>203</v>
@@ -6272,7 +6241,7 @@
       </c>
       <c r="R41" s="5"/>
     </row>
-    <row r="42">
+    <row r="42" spans="1:18">
       <c r="M42" s="7"/>
       <c r="N42" s="7"/>
       <c r="O42" s="7"/>
@@ -6280,7 +6249,7 @@
       <c r="Q42" s="7"/>
       <c r="R42" s="7"/>
     </row>
-    <row r="46">
+    <row r="46" spans="1:18">
       <c r="A46" s="43"/>
       <c r="B46" s="43"/>
       <c r="C46" s="44" t="s">
@@ -6298,7 +6267,7 @@
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
     </row>
-    <row r="47">
+    <row r="47" spans="1:18">
       <c r="A47" s="47" t="s">
         <v>230</v>
       </c>
@@ -6333,16 +6302,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:18">
       <c r="A48" s="51">
-        <v>41.0</v>
+        <v>41</v>
       </c>
       <c r="B48" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C48" s="70"/>
       <c r="D48" s="22">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E48" s="51" t="s">
         <v>235</v>
@@ -6364,16 +6333,16 @@
       </c>
       <c r="R48" s="5"/>
     </row>
-    <row r="49">
+    <row r="49" spans="1:18">
       <c r="A49" s="51">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="B49" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C49" s="70"/>
       <c r="D49" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E49" s="51" t="s">
         <v>236</v>
@@ -6395,16 +6364,16 @@
       </c>
       <c r="R49" s="5"/>
     </row>
-    <row r="50">
+    <row r="50" spans="1:18">
       <c r="A50" s="51">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="B50" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C50" s="70"/>
       <c r="D50" s="22">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="E50" s="51" t="s">
         <v>237</v>
@@ -6426,14 +6395,14 @@
       </c>
       <c r="R50" s="5"/>
     </row>
-    <row r="51">
+    <row r="51" spans="1:18">
       <c r="A51" s="51">
-        <v>44.0</v>
+        <v>44</v>
       </c>
       <c r="B51" s="49"/>
       <c r="C51" s="70"/>
       <c r="D51" s="22">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E51" s="51" t="s">
         <v>235</v>
@@ -6453,14 +6422,14 @@
       </c>
       <c r="R51" s="5"/>
     </row>
-    <row r="52">
+    <row r="52" spans="1:18">
       <c r="A52" s="51">
-        <v>45.0</v>
+        <v>45</v>
       </c>
       <c r="B52" s="49"/>
       <c r="C52" s="70"/>
       <c r="D52" s="22">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="E52" s="51" t="s">
         <v>235</v>
@@ -6480,7 +6449,7 @@
       </c>
       <c r="R52" s="5"/>
     </row>
-    <row r="53">
+    <row r="53" spans="1:18">
       <c r="M53" s="7"/>
       <c r="N53" s="7"/>
       <c r="O53" s="7"/>
@@ -6488,12 +6457,12 @@
       <c r="Q53" s="7"/>
       <c r="R53" s="7"/>
     </row>
-    <row r="104">
+    <row r="104" spans="2:10">
       <c r="B104" s="71"/>
       <c r="C104" s="71"/>
       <c r="D104" s="71"/>
     </row>
-    <row r="105">
+    <row r="105" spans="2:10">
       <c r="E105" s="3"/>
       <c r="F105" s="3"/>
       <c r="G105" s="3"/>
@@ -6502,43 +6471,55 @@
       <c r="J105" s="3"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:J76"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="22.14"/>
-    <col customWidth="1" min="2" max="2" width="15.86"/>
-    <col customWidth="1" min="3" max="3" width="16.0"/>
-    <col customWidth="1" min="4" max="4" width="18.0"/>
-    <col customWidth="1" min="5" max="5" width="29.57"/>
-    <col customWidth="1" min="6" max="6" width="25.29"/>
-    <col customWidth="1" min="7" max="7" width="21.86"/>
-    <col customWidth="1" min="8" max="8" width="51.0"/>
-    <col customWidth="1" min="9" max="9" width="52.86"/>
-    <col customWidth="1" min="10" max="10" width="26.57"/>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="29.5703125" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="51" customWidth="1"/>
+    <col min="9" max="9" width="52.85546875" customWidth="1"/>
+    <col min="10" max="10" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:10">
       <c r="A1" s="15" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:10">
+      <c r="A2" s="78" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="3">
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
@@ -6570,9 +6551,9 @@
         <v>269</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:10">
       <c r="A4" s="22">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="B4" s="22" t="s">
         <v>95</v>
@@ -6581,7 +6562,7 @@
         <v>96</v>
       </c>
       <c r="D4" s="22">
-        <v>7.41258963E9</v>
+        <v>7412589630</v>
       </c>
       <c r="E4" s="22" t="s">
         <v>97</v>
@@ -6596,15 +6577,15 @@
         <v>99</v>
       </c>
       <c r="I4" s="22">
-        <v>411002.0</v>
+        <v>411002</v>
       </c>
       <c r="J4" s="22">
-        <v>456889.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>456889</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="22">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="B5" s="22" t="s">
         <v>100</v>
@@ -6613,7 +6594,7 @@
         <v>101</v>
       </c>
       <c r="D5" s="22">
-        <v>8.56598529E9</v>
+        <v>8565985290</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>102</v>
@@ -6628,15 +6609,15 @@
         <v>104</v>
       </c>
       <c r="I5" s="22">
-        <v>444901.0</v>
+        <v>444901</v>
       </c>
       <c r="J5" s="22">
-        <v>4566789.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>4566789</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="22">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>105</v>
@@ -6645,7 +6626,7 @@
         <v>106</v>
       </c>
       <c r="D6" s="22">
-        <v>9.71938095E9</v>
+        <v>9719380950</v>
       </c>
       <c r="E6" s="22" t="s">
         <v>107</v>
@@ -6660,15 +6641,15 @@
         <v>109</v>
       </c>
       <c r="I6" s="22">
-        <v>413510.0</v>
+        <v>413510</v>
       </c>
       <c r="J6" s="22">
-        <v>8676689.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>8676689</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="22">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="B7" s="22" t="s">
         <v>110</v>
@@ -6677,7 +6658,7 @@
         <v>111</v>
       </c>
       <c r="D7" s="22">
-        <v>9.887277661E9</v>
+        <v>9887277661</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>112</v>
@@ -6692,15 +6673,15 @@
         <v>114</v>
       </c>
       <c r="I7" s="22">
-        <v>41005.0</v>
+        <v>41005</v>
       </c>
       <c r="J7" s="22">
-        <v>1.2786589E7</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>12786589</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="22">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="B8" s="22" t="s">
         <v>115</v>
@@ -6709,7 +6690,7 @@
         <v>116</v>
       </c>
       <c r="D8" s="22">
-        <v>9.902617227E9</v>
+        <v>9902617227</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>117</v>
@@ -6724,13 +6705,13 @@
         <v>119</v>
       </c>
       <c r="I8" s="22">
-        <v>400030.0</v>
+        <v>400030</v>
       </c>
       <c r="J8" s="22">
-        <v>1.6896489E7</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>16896489</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="24"/>
       <c r="B10" s="24"/>
       <c r="C10" s="72" t="s">
@@ -6739,7 +6720,7 @@
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:10">
       <c r="A11" s="73" t="s">
         <v>60</v>
       </c>
@@ -6756,92 +6737,92 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:10">
       <c r="A12" s="22">
-        <v>101.0</v>
+        <v>101</v>
       </c>
       <c r="B12" s="22">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="C12" s="29">
-        <v>12500.0</v>
+        <v>12500</v>
       </c>
       <c r="D12" s="29">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="30">
-        <v>44896.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>44896</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="22">
-        <v>102.0</v>
+        <v>102</v>
       </c>
       <c r="B13" s="22">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="C13" s="29">
-        <v>15600.0</v>
+        <v>15600</v>
       </c>
       <c r="D13" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="22" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:10">
       <c r="A14" s="22">
-        <v>103.0</v>
+        <v>103</v>
       </c>
       <c r="B14" s="22">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="C14" s="22">
-        <v>6000.0</v>
+        <v>6000</v>
       </c>
       <c r="D14" s="22">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E14" s="22" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:10">
       <c r="A15" s="22">
-        <v>104.0</v>
+        <v>104</v>
       </c>
       <c r="B15" s="22">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="C15" s="22">
-        <v>22750.0</v>
+        <v>22750</v>
       </c>
       <c r="D15" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="22" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:10">
       <c r="A16" s="22">
-        <v>105.0</v>
+        <v>105</v>
       </c>
       <c r="B16" s="22">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="C16" s="22">
-        <v>44560.0</v>
+        <v>44560</v>
       </c>
       <c r="D16" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="22" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:9">
       <c r="A18" s="24"/>
       <c r="B18" s="24"/>
       <c r="C18" s="24"/>
@@ -6854,7 +6835,7 @@
       <c r="H18" s="24"/>
       <c r="I18" s="24"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:9">
       <c r="A19" s="32" t="s">
         <v>69</v>
       </c>
@@ -6883,15 +6864,15 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:9">
       <c r="A20" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B20" s="22">
-        <v>101.0</v>
+        <v>101</v>
       </c>
       <c r="C20" s="22">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="D20" s="22" t="s">
         <v>125</v>
@@ -6906,21 +6887,21 @@
         <v>126</v>
       </c>
       <c r="H20" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="I20" s="22" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:9">
       <c r="A21" s="22">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B21" s="22">
-        <v>101.0</v>
+        <v>101</v>
       </c>
       <c r="C21" s="22">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="D21" s="22" t="s">
         <v>125</v>
@@ -6935,21 +6916,21 @@
         <v>126</v>
       </c>
       <c r="H21" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="22" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:9">
       <c r="A22" s="22">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B22" s="22">
-        <v>101.0</v>
+        <v>101</v>
       </c>
       <c r="C22" s="22">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="D22" s="22" t="s">
         <v>125</v>
@@ -6964,21 +6945,21 @@
         <v>126</v>
       </c>
       <c r="H22" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="22" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:9">
       <c r="A23" s="22">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B23" s="22">
-        <v>102.0</v>
+        <v>102</v>
       </c>
       <c r="C23" s="22">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="D23" s="22" t="s">
         <v>128</v>
@@ -6993,21 +6974,21 @@
         <v>129</v>
       </c>
       <c r="H23" s="22">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I23" s="22" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:9">
       <c r="A24" s="22">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B24" s="22">
-        <v>102.0</v>
+        <v>102</v>
       </c>
       <c r="C24" s="22">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="D24" s="22" t="s">
         <v>128</v>
@@ -7022,21 +7003,21 @@
         <v>129</v>
       </c>
       <c r="H24" s="22">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I24" s="22" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:9">
       <c r="A25" s="22">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B25" s="22">
-        <v>103.0</v>
+        <v>103</v>
       </c>
       <c r="C25" s="22">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="D25" s="22" t="s">
         <v>132</v>
@@ -7051,21 +7032,21 @@
         <v>135</v>
       </c>
       <c r="H25" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="I25" s="22" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:9">
       <c r="A26" s="22">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B26" s="22">
-        <v>104.0</v>
+        <v>104</v>
       </c>
       <c r="C26" s="22">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="D26" s="22" t="s">
         <v>136</v>
@@ -7080,21 +7061,21 @@
         <v>137</v>
       </c>
       <c r="H26" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="I26" s="22" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:9">
       <c r="A27" s="22">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B27" s="22">
-        <v>104.0</v>
+        <v>104</v>
       </c>
       <c r="C27" s="22">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="D27" s="22" t="s">
         <v>136</v>
@@ -7109,21 +7090,21 @@
         <v>137</v>
       </c>
       <c r="H27" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="I27" s="22" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:9">
       <c r="A28" s="22">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B28" s="22">
-        <v>105.0</v>
+        <v>105</v>
       </c>
       <c r="C28" s="22">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="D28" s="22" t="s">
         <v>140</v>
@@ -7132,19 +7113,19 @@
         <v>141</v>
       </c>
       <c r="F28" s="30">
-        <v>44564.0</v>
+        <v>44564</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>141</v>
       </c>
       <c r="H28" s="22">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="I28" s="22" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:6">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="66" t="s">
@@ -7154,7 +7135,7 @@
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:6">
       <c r="A38" s="3" t="s">
         <v>1</v>
       </c>
@@ -7174,7 +7155,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:6">
       <c r="A39" s="4" t="s">
         <v>60</v>
       </c>
@@ -7194,7 +7175,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:6">
       <c r="A40" s="4" t="s">
         <v>7</v>
       </c>
@@ -7212,7 +7193,7 @@
       </c>
       <c r="F40" s="5"/>
     </row>
-    <row r="41">
+    <row r="41" spans="1:6">
       <c r="A41" s="4" t="s">
         <v>62</v>
       </c>
@@ -7228,7 +7209,7 @@
       </c>
       <c r="F41" s="5"/>
     </row>
-    <row r="42">
+    <row r="42" spans="1:6">
       <c r="A42" s="4" t="s">
         <v>64</v>
       </c>
@@ -7244,7 +7225,7 @@
       </c>
       <c r="F42" s="5"/>
     </row>
-    <row r="43">
+    <row r="43" spans="1:6">
       <c r="A43" s="4" t="s">
         <v>65</v>
       </c>
@@ -7260,7 +7241,7 @@
       </c>
       <c r="F43" s="5"/>
     </row>
-    <row r="44">
+    <row r="44" spans="1:6">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -7268,17 +7249,17 @@
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
     </row>
-    <row r="45">
+    <row r="45" spans="1:6">
       <c r="B45" s="15" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:6">
       <c r="C46" s="15" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:6">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="66" t="s">
@@ -7288,7 +7269,7 @@
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
     </row>
-    <row r="50">
+    <row r="50" spans="1:6">
       <c r="A50" s="3" t="s">
         <v>1</v>
       </c>
@@ -7308,7 +7289,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:6">
       <c r="A51" s="4" t="s">
         <v>69</v>
       </c>
@@ -7328,7 +7309,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:6">
       <c r="A52" s="4" t="s">
         <v>60</v>
       </c>
@@ -7346,7 +7327,7 @@
       </c>
       <c r="F52" s="5"/>
     </row>
-    <row r="53">
+    <row r="53" spans="1:6">
       <c r="A53" s="4" t="s">
         <v>46</v>
       </c>
@@ -7364,7 +7345,7 @@
       </c>
       <c r="F53" s="5"/>
     </row>
-    <row r="54">
+    <row r="54" spans="1:6">
       <c r="A54" s="4" t="s">
         <v>72</v>
       </c>
@@ -7380,7 +7361,7 @@
       </c>
       <c r="F54" s="5"/>
     </row>
-    <row r="55">
+    <row r="55" spans="1:6">
       <c r="A55" s="4" t="s">
         <v>73</v>
       </c>
@@ -7394,7 +7375,7 @@
       </c>
       <c r="F55" s="5"/>
     </row>
-    <row r="56">
+    <row r="56" spans="1:6">
       <c r="A56" s="4" t="s">
         <v>75</v>
       </c>
@@ -7410,7 +7391,7 @@
       </c>
       <c r="F56" s="5"/>
     </row>
-    <row r="57">
+    <row r="57" spans="1:6">
       <c r="A57" s="4" t="s">
         <v>76</v>
       </c>
@@ -7424,7 +7405,7 @@
       </c>
       <c r="F57" s="5"/>
     </row>
-    <row r="58">
+    <row r="58" spans="1:6">
       <c r="A58" s="4" t="s">
         <v>77</v>
       </c>
@@ -7440,7 +7421,7 @@
       </c>
       <c r="F58" s="5"/>
     </row>
-    <row r="59">
+    <row r="59" spans="1:6">
       <c r="A59" s="4" t="s">
         <v>78</v>
       </c>
@@ -7456,7 +7437,7 @@
       </c>
       <c r="F59" s="5"/>
     </row>
-    <row r="60">
+    <row r="60" spans="1:6">
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
@@ -7464,7 +7445,7 @@
       <c r="E60" s="7"/>
       <c r="F60" s="7"/>
     </row>
-    <row r="64">
+    <row r="64" spans="1:6">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="66" t="s">
@@ -7474,7 +7455,7 @@
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
     </row>
-    <row r="65">
+    <row r="65" spans="1:6">
       <c r="A65" s="3" t="s">
         <v>1</v>
       </c>
@@ -7494,7 +7475,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:6">
       <c r="A66" s="4" t="s">
         <v>7</v>
       </c>
@@ -7514,7 +7495,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:6">
       <c r="A67" s="4" t="s">
         <v>12</v>
       </c>
@@ -7530,7 +7511,7 @@
       </c>
       <c r="F67" s="5"/>
     </row>
-    <row r="68">
+    <row r="68" spans="1:6">
       <c r="A68" s="4" t="s">
         <v>14</v>
       </c>
@@ -7546,7 +7527,7 @@
       </c>
       <c r="F68" s="5"/>
     </row>
-    <row r="69">
+    <row r="69" spans="1:6">
       <c r="A69" s="4" t="s">
         <v>15</v>
       </c>
@@ -7564,7 +7545,7 @@
       </c>
       <c r="F69" s="5"/>
     </row>
-    <row r="70">
+    <row r="70" spans="1:6">
       <c r="A70" s="4" t="s">
         <v>19</v>
       </c>
@@ -7582,7 +7563,7 @@
       </c>
       <c r="F70" s="5"/>
     </row>
-    <row r="71">
+    <row r="71" spans="1:6">
       <c r="A71" s="4" t="s">
         <v>21</v>
       </c>
@@ -7598,7 +7579,7 @@
       </c>
       <c r="F71" s="5"/>
     </row>
-    <row r="72">
+    <row r="72" spans="1:6">
       <c r="A72" s="4" t="s">
         <v>22</v>
       </c>
@@ -7614,7 +7595,7 @@
       </c>
       <c r="F72" s="5"/>
     </row>
-    <row r="73">
+    <row r="73" spans="1:6">
       <c r="A73" s="4" t="s">
         <v>23</v>
       </c>
@@ -7630,7 +7611,7 @@
       </c>
       <c r="F73" s="5"/>
     </row>
-    <row r="74">
+    <row r="74" spans="1:6">
       <c r="A74" s="4" t="s">
         <v>25</v>
       </c>
@@ -7646,7 +7627,7 @@
       </c>
       <c r="F74" s="5"/>
     </row>
-    <row r="75">
+    <row r="75" spans="1:6">
       <c r="A75" s="4" t="s">
         <v>269</v>
       </c>
@@ -7664,7 +7645,7 @@
       </c>
       <c r="F75" s="5"/>
     </row>
-    <row r="76">
+    <row r="76" spans="1:6">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
@@ -7676,6 +7657,6 @@
   <mergeCells count="1">
     <mergeCell ref="A2:J2"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>